<commit_message>
add all 12 tab
</commit_message>
<xml_diff>
--- a/output/groupings_dems_impeachment_0927.xlsx
+++ b/output/groupings_dems_impeachment_0927.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kessler\GitHub_Kessler\cnn_impeachment_tallies\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5927971-5BBD-4805-92BD-D592E6C73308}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8219E6A8-3C24-42E6-ADB1-B8564DFEA26E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24660" yWindow="1395" windowWidth="12915" windowHeight="18330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list_of_NOs" sheetId="12" r:id="rId1"/>
@@ -1189,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49D55FB-2331-4117-B18D-660613BB1D8F}">
   <dimension ref="A1:AP13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3175,8 +3175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>